<commit_message>
new version with disordered matrix
</commit_message>
<xml_diff>
--- a/doc/data1.xlsx
+++ b/doc/data1.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proj\fermi_hubbard_commutators\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC60C406-3971-4A6B-9066-4911942BE524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609C4EDC-35EE-4862-88A9-9D1A58CD5D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$82</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Index0</t>
   </si>
@@ -58,6 +55,10 @@
   <si>
     <t>Err</t>
   </si>
+  <si>
+    <t>diff</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -78,35 +79,29 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,48 +124,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="差" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -468,11 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -499,11 +483,14 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -525,7 +512,7 @@
       <c r="G2">
         <v>0.15044269792543619</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>0.15044269792543619</v>
       </c>
       <c r="I2">
@@ -533,7 +520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>0</v>
       </c>
@@ -555,10 +542,10 @@
       <c r="G3">
         <v>0.48078973319345569</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>0.48078973319345569</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="0">G3-H3</f>
         <v>0</v>
       </c>
@@ -585,15 +572,15 @@
       <c r="G4">
         <v>0.15503469264195471</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>0.15503469264195471</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>0</v>
       </c>
@@ -615,15 +602,15 @@
       <c r="G5">
         <v>7.4222561305436627E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>7.4222561305436627E-2</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>0</v>
       </c>
@@ -645,10 +632,10 @@
       <c r="G6">
         <v>0.38182342860530483</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>0.38182342860530483</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -675,10 +662,10 @@
       <c r="G7">
         <v>0.13862522445687631</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>0.13862522445687631</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -705,12 +692,12 @@
       <c r="G8">
         <v>5.9011769571893302E-2</v>
       </c>
-      <c r="H8">
-        <v>5.8698198336275598E-2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>3.135712356177045E-4</v>
+      <c r="H8" s="3">
+        <v>5.9011769571893302E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -735,15 +722,15 @@
       <c r="G9">
         <v>0.37534585913409291</v>
       </c>
-      <c r="H9">
-        <v>0.39091928409939902</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.5573424965306115E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H9" s="3">
+        <v>0.37534585913409291</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>0</v>
       </c>
@@ -765,15 +752,15 @@
       <c r="G10">
         <v>0.13862522445687631</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>0.13862522445687631</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>0</v>
       </c>
@@ -795,15 +782,15 @@
       <c r="G11">
         <v>9.1261100202069567E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>9.1261100202069567E-2</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>0</v>
       </c>
@@ -825,10 +812,10 @@
       <c r="G12">
         <v>0.25748850616950852</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>0.25748850616950852</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -855,15 +842,15 @@
       <c r="G13">
         <v>7.7809298867654669E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>7.7809298867654669E-2</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>0</v>
       </c>
@@ -885,15 +872,15 @@
       <c r="G14">
         <v>0.23590581267047059</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>0.23590581267047059</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>0</v>
       </c>
@@ -915,10 +902,10 @@
       <c r="G15">
         <v>1.0090109249730319</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>1.0090109249730319</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -945,10 +932,10 @@
       <c r="G16">
         <v>0.40857843070540911</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>0.40857843070540911</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -975,12 +962,12 @@
       <c r="G17">
         <v>0.14622467824104179</v>
       </c>
-      <c r="H17">
-        <v>0.15248763467627111</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="0"/>
-        <v>-6.262956435229311E-3</v>
+      <c r="H17" s="3">
+        <v>0.14622467824104179</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
@@ -1005,15 +992,15 @@
       <c r="G18">
         <v>0.37144768752139229</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>0.37144768752139229</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1035,10 +1022,10 @@
       <c r="G19">
         <v>0.26273551101220721</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>0.26273551101220721</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1065,12 +1052,12 @@
       <c r="G20">
         <v>9.1261100202069581E-2</v>
       </c>
-      <c r="H20">
-        <v>8.100537894677115E-2</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>1.0255721255298431E-2</v>
+      <c r="H20" s="3">
+        <v>9.1261100202069581E-2</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
@@ -1095,15 +1082,15 @@
       <c r="G21">
         <v>0.37932953021254728</v>
       </c>
-      <c r="H21">
-        <v>0.34232242114150868</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>3.7007109071038602E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H21" s="3">
+        <v>0.37932953021254728</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1125,12 +1112,12 @@
       <c r="G22">
         <v>6.9147338684785634E-2</v>
       </c>
-      <c r="H22">
-        <v>6.4532887797314142E-2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>4.6144508874714912E-3</v>
+      <c r="H22" s="3">
+        <v>0.1014316181718193</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="0"/>
+        <v>-3.2284279487033662E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
@@ -1155,12 +1142,12 @@
       <c r="G23">
         <v>0.17759304940463491</v>
       </c>
-      <c r="H23">
-        <v>0.17515841996320139</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>2.4346294414335223E-3</v>
+      <c r="H23" s="3">
+        <v>0.17759304940463491</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
@@ -1185,15 +1172,15 @@
       <c r="G24">
         <v>0.48557794993019049</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>0.48557794993019049</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1215,15 +1202,15 @@
       <c r="G25">
         <v>0.1554914037058073</v>
       </c>
-      <c r="H25">
-        <v>0.1554914037058073</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H25" s="3">
+        <v>0.24585349614354859</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.0362092437741293E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1245,15 +1232,15 @@
       <c r="G26">
         <v>5.143427698142905E-2</v>
       </c>
-      <c r="H26">
-        <v>5.3033332421187747E-2</v>
-      </c>
-      <c r="I26" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.5990554397586967E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H26" s="3">
+        <v>5.143427698142905E-2</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1275,15 +1262,15 @@
       <c r="G27">
         <v>0.20690108531469781</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>0.20690108531469781</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1305,10 +1292,10 @@
       <c r="G28">
         <v>0.1231422216343093</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>0.1231422216343093</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1335,10 +1322,10 @@
       <c r="G29">
         <v>0.60177079170174486</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>0.60177079170174486</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1365,15 +1352,15 @@
       <c r="G30">
         <v>0.9615794663869115</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="3">
         <v>0.9615794663869115</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1395,10 +1382,10 @@
       <c r="G31">
         <v>0.31006938528390943</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="3">
         <v>0.31006938528390943</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1425,12 +1412,12 @@
       <c r="G32">
         <v>0.25595314218121668</v>
       </c>
-      <c r="H32">
-        <v>0.2475355162397489</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="0"/>
-        <v>8.4176259414677768E-3</v>
+      <c r="H32" s="3">
+        <v>0.25595314218121668</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
@@ -1455,15 +1442,15 @@
       <c r="G33">
         <v>1.54185227084198</v>
       </c>
-      <c r="H33">
-        <v>1.535463380223913</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="0"/>
-        <v>6.3888906180669114E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H33" s="3">
+        <v>1.54185227084198</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>0</v>
       </c>
@@ -1485,15 +1472,15 @@
       <c r="G34">
         <v>0.26123436741248968</v>
       </c>
-      <c r="H34">
-        <v>0.2647388271386204</v>
-      </c>
-      <c r="I34" s="2">
-        <f t="shared" si="0"/>
-        <v>-3.5044597261307264E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H34" s="3">
+        <v>0.42575063584803702</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.16451626843554734</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>0</v>
       </c>
@@ -1515,15 +1502,15 @@
       <c r="G35">
         <v>0</v>
       </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>0</v>
       </c>
@@ -1545,15 +1532,15 @@
       <c r="G36">
         <v>0</v>
       </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H36" s="3">
+        <v>0.40550978852759578</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.40550978852759578</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>0</v>
       </c>
@@ -1575,12 +1562,12 @@
       <c r="G37">
         <v>0</v>
       </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H37" s="3">
+        <v>0.27725044891375261</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.27725044891375261</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
@@ -1605,12 +1592,12 @@
       <c r="G38">
         <v>0.31875693963451712</v>
       </c>
-      <c r="H38">
-        <v>0.30651063125284822</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="0"/>
-        <v>1.2246308381668902E-2</v>
+      <c r="H38" s="3">
+        <v>0.31875693963451712</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
@@ -1635,15 +1622,15 @@
       <c r="G39">
         <v>0.82656976318896291</v>
       </c>
-      <c r="H39">
-        <v>0.82136400882646432</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="0"/>
-        <v>5.2057543624985936E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H39" s="3">
+        <v>0.82656976318896291</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>0</v>
       </c>
@@ -1665,12 +1652,12 @@
       <c r="G40">
         <v>0.13351229366568959</v>
       </c>
-      <c r="H40">
-        <v>0.12951227262575579</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="0"/>
-        <v>4.0000210399337988E-3</v>
+      <c r="H40" s="3">
+        <v>0.19719796406907009</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="0"/>
+        <v>-6.3685670403380495E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
@@ -1695,10 +1682,10 @@
       <c r="G41">
         <v>0.34583996015276519</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="3">
         <v>0.34583996015276519</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1725,15 +1712,15 @@
       <c r="G42">
         <v>1.9553020136549459</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="3">
         <v>1.9553020136549459</v>
       </c>
-      <c r="I42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I42" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>0</v>
       </c>
@@ -1755,15 +1742,15 @@
       <c r="G43">
         <v>0.38928146268019792</v>
       </c>
-      <c r="H43">
-        <v>0.38928146268019792</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H43" s="3">
+        <v>0.6155080364756299</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.22622657379543198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>0</v>
       </c>
@@ -1785,15 +1772,15 @@
       <c r="G44">
         <v>7.3043075915682182E-2</v>
       </c>
-      <c r="H44">
-        <v>7.4056305045655996E-2</v>
-      </c>
-      <c r="I44" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.0132291299738139E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H44" s="3">
+        <v>9.1122244820770679E-2</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.8079168905088497E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>0</v>
       </c>
@@ -1815,15 +1802,15 @@
       <c r="G45">
         <v>0.16454660220669459</v>
       </c>
-      <c r="H45">
-        <v>0.16454660220669459</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H45" s="3">
+        <v>0.24681990331004189</v>
+      </c>
+      <c r="I45" s="3">
+        <f t="shared" si="0"/>
+        <v>-8.2273301103347296E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>0</v>
       </c>
@@ -1845,15 +1832,15 @@
       <c r="G46">
         <v>0.1168950294871952</v>
       </c>
-      <c r="H46">
-        <v>0.1168950294871952</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H46" s="3">
+        <v>0.3408046468431789</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.22390961735598369</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>0</v>
       </c>
@@ -1875,15 +1862,15 @@
       <c r="G47">
         <v>0</v>
       </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>0</v>
       </c>
@@ -1905,15 +1892,15 @@
       <c r="G48">
         <v>0</v>
       </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>0</v>
       </c>
@@ -1935,15 +1922,15 @@
       <c r="G49">
         <v>0</v>
       </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>0</v>
       </c>
@@ -1965,15 +1952,15 @@
       <c r="G50">
         <v>5.2182181505022497E-2</v>
       </c>
-      <c r="H50">
-        <v>5.3473194813464811E-2</v>
-      </c>
-      <c r="I50" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.2910133084423139E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H50" s="3">
+        <v>5.2182181505022497E-2</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>0</v>
       </c>
@@ -1995,15 +1982,15 @@
       <c r="G51">
         <v>0.64235924882592887</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="3">
         <v>0.64235924882592887</v>
       </c>
-      <c r="I51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I51" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>0</v>
       </c>
@@ -2025,15 +2012,15 @@
       <c r="G52">
         <v>7.7745701852903651E-2</v>
       </c>
-      <c r="H52">
-        <v>7.7745701852903651E-2</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H52" s="3">
+        <v>0.1229267480717743</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="0"/>
+        <v>-4.5181046218870646E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>0</v>
       </c>
@@ -2055,15 +2042,15 @@
       <c r="G53">
         <v>5.8976453167617682E-2</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="3">
         <v>5.8976453167617682E-2</v>
       </c>
-      <c r="I53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I53" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>0</v>
       </c>
@@ -2085,15 +2072,15 @@
       <c r="G54">
         <v>9.6391462139348377E-2</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="3">
         <v>9.6391462139348377E-2</v>
       </c>
-      <c r="I54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I54" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>0</v>
       </c>
@@ -2115,10 +2102,10 @@
       <c r="G55">
         <v>5.6746868810851822E-2</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="3">
         <v>5.6746868810851822E-2</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2145,12 +2132,12 @@
       <c r="G56">
         <v>0.24074530322993859</v>
       </c>
-      <c r="H56">
-        <v>0.2279440396578756</v>
-      </c>
-      <c r="I56">
-        <f t="shared" si="0"/>
-        <v>1.2801263572062987E-2</v>
+      <c r="H56" s="3">
+        <v>0.24074530322993859</v>
+      </c>
+      <c r="I56" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.15">
@@ -2175,15 +2162,15 @@
       <c r="G57">
         <v>0.70641057930978268</v>
       </c>
-      <c r="H57">
-        <v>0.69839983094648816</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="0"/>
-        <v>8.0107483632945176E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H57" s="3">
+        <v>0.70641057930978268</v>
+      </c>
+      <c r="I57" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>1</v>
       </c>
@@ -2205,12 +2192,12 @@
       <c r="G58">
         <v>0.13791572489154691</v>
       </c>
-      <c r="H58">
-        <v>0.13791572489154691</v>
-      </c>
-      <c r="I58">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H58" s="3">
+        <v>0.20254096196088989</v>
+      </c>
+      <c r="I58" s="3">
+        <f t="shared" si="0"/>
+        <v>-6.4625237069342978E-2</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.15">
@@ -2235,12 +2222,12 @@
       <c r="G59">
         <v>0.1750599906925103</v>
       </c>
-      <c r="H59">
-        <v>0.17445669136423961</v>
-      </c>
-      <c r="I59">
-        <f t="shared" si="0"/>
-        <v>6.0329932827068999E-4</v>
+      <c r="H59" s="3">
+        <v>0.1750599906925103</v>
+      </c>
+      <c r="I59" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.15">
@@ -2265,15 +2252,15 @@
       <c r="G60">
         <v>1.355343459456106</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="3">
         <v>1.355343459456106</v>
       </c>
-      <c r="I60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I60" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>1</v>
       </c>
@@ -2295,15 +2282,15 @@
       <c r="G61">
         <v>0.26386955909865728</v>
       </c>
-      <c r="H61">
-        <v>0.26386955909865728</v>
-      </c>
-      <c r="I61">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H61" s="3">
+        <v>0.41721440596808212</v>
+      </c>
+      <c r="I61" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.15334484686942484</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>1</v>
       </c>
@@ -2325,15 +2312,15 @@
       <c r="G62">
         <v>2.1830861641848359E-2</v>
       </c>
-      <c r="H62">
-        <v>2.4610809355871208E-2</v>
-      </c>
-      <c r="I62" s="2">
-        <f t="shared" si="0"/>
-        <v>-2.7799477140228492E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H62" s="3">
+        <v>3.2812420894433897E-2</v>
+      </c>
+      <c r="I62" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.0981559252585538E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>1</v>
       </c>
@@ -2355,15 +2342,15 @@
       <c r="G63">
         <v>0.2443842381973825</v>
       </c>
-      <c r="H63">
-        <v>0.2443842381973825</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H63" s="3">
+        <v>0.30548029774672802</v>
+      </c>
+      <c r="I63" s="3">
+        <f t="shared" si="0"/>
+        <v>-6.1096059549345522E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>1</v>
       </c>
@@ -2385,12 +2372,12 @@
       <c r="G64">
         <v>6.5967389774664334E-2</v>
       </c>
-      <c r="H64">
-        <v>6.5967389774664334E-2</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H64" s="3">
+        <v>0.19232633820228881</v>
+      </c>
+      <c r="I64" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.12635894842762446</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.15">
@@ -2415,12 +2402,12 @@
       <c r="G65">
         <v>0.35855791788305619</v>
       </c>
-      <c r="H65">
-        <v>0.35734601916438019</v>
-      </c>
-      <c r="I65">
-        <f t="shared" si="0"/>
-        <v>1.2118987186759966E-3</v>
+      <c r="H65" s="3">
+        <v>0.35855791788305619</v>
+      </c>
+      <c r="I65" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.15">
@@ -2445,15 +2432,15 @@
       <c r="G66">
         <v>1.0299540246780341</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="3">
         <v>1.0299540246780341</v>
       </c>
-      <c r="I66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="I66" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>1</v>
       </c>
@@ -2475,12 +2462,12 @@
       <c r="G67">
         <v>0.16794986322922811</v>
       </c>
-      <c r="H67">
-        <v>0.16794986322922811</v>
-      </c>
-      <c r="I67">
+      <c r="H67" s="3">
+        <v>0.26555205025906142</v>
+      </c>
+      <c r="I67" s="3">
         <f t="shared" ref="I67:I82" si="1">G67-H67</f>
-        <v>0</v>
+        <v>-9.7602187029833309E-2</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.15">
@@ -2505,10 +2492,10 @@
       <c r="G68">
         <v>0.39684531957557212</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="3">
         <v>0.39684531957557212</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2535,15 +2522,15 @@
       <c r="G69">
         <v>3.7101980489622828</v>
       </c>
-      <c r="H69">
-        <v>3.8297614468479142</v>
-      </c>
-      <c r="I69" s="2">
+      <c r="H69" s="3">
+        <v>3.7101980489622828</v>
+      </c>
+      <c r="I69" s="3">
         <f t="shared" si="1"/>
-        <v>-0.11956339788563142</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>1</v>
       </c>
@@ -2565,15 +2552,15 @@
       <c r="G70">
         <v>0.81896739412600672</v>
       </c>
-      <c r="H70">
+      <c r="H70" s="3">
         <v>0.81896739412600672</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>1</v>
       </c>
@@ -2595,15 +2582,15 @@
       <c r="G71">
         <v>0</v>
       </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71">
+      <c r="H71" s="3">
+        <v>0.10496655283221699</v>
+      </c>
+      <c r="I71" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+        <v>-0.10496655283221699</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>1</v>
       </c>
@@ -2625,15 +2612,15 @@
       <c r="G72">
         <v>0</v>
       </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
+      <c r="H72" s="3">
+        <v>0</v>
+      </c>
+      <c r="I72" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>1</v>
       </c>
@@ -2655,15 +2642,15 @@
       <c r="G73">
         <v>0</v>
       </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73">
+      <c r="H73" s="3">
+        <v>0.50352429010936051</v>
+      </c>
+      <c r="I73" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+        <v>-0.50352429010936051</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>1</v>
       </c>
@@ -2685,15 +2672,15 @@
       <c r="G74">
         <v>9.4722366144563336E-2</v>
       </c>
-      <c r="H74">
-        <v>0.1021843814694807</v>
-      </c>
-      <c r="I74" s="2">
+      <c r="H74" s="3">
+        <v>9.4722366144563336E-2</v>
+      </c>
+      <c r="I74" s="3">
         <f t="shared" si="1"/>
-        <v>-7.4620153249173593E-3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>1</v>
       </c>
@@ -2715,15 +2702,15 @@
       <c r="G75">
         <v>0.12874425308475421</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="3">
         <v>0.12874425308475421</v>
       </c>
-      <c r="I75">
+      <c r="I75" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>1</v>
       </c>
@@ -2745,15 +2732,15 @@
       <c r="G76">
         <v>3.8904649433827342E-2</v>
       </c>
-      <c r="H76">
-        <v>3.8904649433827342E-2</v>
-      </c>
-      <c r="I76">
+      <c r="H76" s="3">
+        <v>6.1513651890637323E-2</v>
+      </c>
+      <c r="I76" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+        <v>-2.2609002456809982E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>1</v>
       </c>
@@ -2775,15 +2762,15 @@
       <c r="G77">
         <v>0</v>
       </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77">
+      <c r="H77" s="3">
+        <v>0</v>
+      </c>
+      <c r="I77" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>1</v>
       </c>
@@ -2805,15 +2792,15 @@
       <c r="G78">
         <v>0</v>
       </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78">
+      <c r="H78" s="3">
+        <v>0</v>
+      </c>
+      <c r="I78" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>1</v>
       </c>
@@ -2835,15 +2822,15 @@
       <c r="G79">
         <v>0</v>
       </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79">
+      <c r="H79" s="3">
+        <v>0</v>
+      </c>
+      <c r="I79" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>1</v>
       </c>
@@ -2865,15 +2852,15 @@
       <c r="G80">
         <v>2.9488226583808841E-2</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="3">
         <v>2.9488226583808841E-2</v>
       </c>
-      <c r="I80">
+      <c r="I80" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>1</v>
       </c>
@@ -2895,15 +2882,15 @@
       <c r="G81">
         <v>0.2198473726262502</v>
       </c>
-      <c r="H81">
-        <v>0.1958422121290237</v>
-      </c>
-      <c r="I81">
+      <c r="H81" s="3">
+        <v>0.2198473726262502</v>
+      </c>
+      <c r="I81" s="3">
         <f t="shared" si="1"/>
-        <v>2.4005160497226508E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>1</v>
       </c>
@@ -2925,24 +2912,16 @@
       <c r="G82">
         <v>6.3271756749900404E-2</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="3">
         <v>6.3271756749900404E-2</v>
       </c>
-      <c r="I82">
+      <c r="I82" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F82" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>